<commit_message>
Review intro and Section 1
</commit_message>
<xml_diff>
--- a/data/export/rmse_graphs/rmse_graphs.xlsx
+++ b/data/export/rmse_graphs/rmse_graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexmoran/Desktop/thesis/data/export/rmse_graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342C1F19-6922-3F4C-BBC1-6DD0847C955C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{79AAD27C-2D69-4944-85D3-20AD7D9660D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="820" windowWidth="27640" windowHeight="16800" activeTab="2" xr2:uid="{0F3A2CF4-6689-C543-B2F2-8F95BC64D9C6}"/>
+    <workbookView xWindow="6580" yWindow="820" windowWidth="27640" windowHeight="16800" activeTab="1" xr2:uid="{0F3A2CF4-6689-C543-B2F2-8F95BC64D9C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Average" sheetId="1" r:id="rId1"/>
@@ -41,19 +41,19 @@
     <t>date</t>
   </si>
   <si>
-    <t>arima</t>
+    <t>ARIMA</t>
   </si>
   <si>
-    <t>forest</t>
+    <t>Optimized forest</t>
   </si>
   <si>
-    <t>mean</t>
+    <t>"Base" forest</t>
   </si>
   <si>
-    <t>ar1</t>
+    <t>AR(1)</t>
   </si>
   <si>
-    <t>naive</t>
+    <t>Naïve</t>
   </si>
 </sst>
 </file>
@@ -143,7 +143,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>arima</c:v>
+                  <c:v>ARIMA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1640,7 +1640,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>forest</c:v>
+                  <c:v>Optimized forest</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3137,7 +3137,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mean</c:v>
+                  <c:v>"Base" forest</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4638,7 +4638,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ar1</c:v>
+                  <c:v>AR(1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6139,7 +6139,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>naive</c:v>
+                  <c:v>Naïve</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7861,7 +7861,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>arima</c:v>
+                  <c:v>ARIMA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9358,7 +9358,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>forest</c:v>
+                  <c:v>Optimized forest</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10855,7 +10855,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mean</c:v>
+                  <c:v>"Base" forest</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12356,7 +12356,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ar1</c:v>
+                  <c:v>AR(1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -13857,7 +13857,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>naive</c:v>
+                  <c:v>Naïve</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -17032,7 +17032,7 @@
   <dimension ref="A1:F242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A243" sqref="A243:XFD243"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21886,8 +21886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{684A923F-B4A0-0F43-9533-1BA8B3F421DF}">
   <dimension ref="A1:F242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A243" sqref="A243:XFD243"/>
+    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26741,7 +26741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD013ADF-505A-E94B-A28C-57188D93A47B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H20" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView topLeftCell="H24" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add Appendix 4, make tables relative
</commit_message>
<xml_diff>
--- a/data/export/rmse_graphs/rmse_graphs.xlsx
+++ b/data/export/rmse_graphs/rmse_graphs.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexmoran/Desktop/thesis/data/export/rmse_graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D83CF7B-E9F9-2140-904A-E0F70CB66D70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0283D486-4201-CA49-8FFB-4524C771E5C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="1200" windowWidth="27640" windowHeight="16800" activeTab="3" xr2:uid="{0F3A2CF4-6689-C543-B2F2-8F95BC64D9C6}"/>
+    <workbookView xWindow="4520" yWindow="1200" windowWidth="27640" windowHeight="16800" activeTab="5" xr2:uid="{0F3A2CF4-6689-C543-B2F2-8F95BC64D9C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Average" sheetId="1" r:id="rId1"/>
     <sheet name="Cumulative" sheetId="2" r:id="rId2"/>
     <sheet name="Graphs" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Table 1" sheetId="5" r:id="rId4"/>
+    <sheet name="Table 2" sheetId="6" r:id="rId5"/>
+    <sheet name="Table 5" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="31">
   <si>
     <t>date</t>
   </si>
@@ -68,12 +70,78 @@
   <si>
     <t>VAR</t>
   </si>
+  <si>
+    <t>TABLE 1</t>
+  </si>
+  <si>
+    <t>Fit and forecast results on simulated AR(1) time series</t>
+  </si>
+  <si>
+    <t>Model Type</t>
+  </si>
+  <si>
+    <t>ARIMA(AIC)</t>
+  </si>
+  <si>
+    <t>Base Tree</t>
+  </si>
+  <si>
+    <t>Hybrid Tree</t>
+  </si>
+  <si>
+    <t>Modified Tree</t>
+  </si>
+  <si>
+    <t>Fit RMSE</t>
+  </si>
+  <si>
+    <t>Forecast RMSE</t>
+  </si>
+  <si>
+    <t>Notes: The first column refers to the ARIMA function optimized by AIC; the last three columns refer to different types of trees: the base tree defined in Section 1, the hybrid tree which borrows the objective function from the base tree but predicts based on an AR(1) assumption, and the modified tree which uses an AR(1) objective function as well as an AR(1) prediction. The first row refers to the in-sample fit provided by each model; the last row refers to an out-of-sample one-period ahead forecast on the last 100 observations generated, in a time series of 511 observations. The lowest RMSE in each row is bolded.</t>
+  </si>
+  <si>
+    <t>Naive</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
+  </si>
+  <si>
+    <t>Fit</t>
+  </si>
+  <si>
+    <t>Forecast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numbers refer to the RMSE generated from each model, divided by the RMSE provided by the naïve model. </t>
+  </si>
+  <si>
+    <t>For the actual RMSEs, see Appendix 4.</t>
+  </si>
+  <si>
+    <t>TABLE 2</t>
+  </si>
+  <si>
+    <t>RMSE Forecast results on US monthly inflation data, January 1999 – January 2020</t>
+  </si>
+  <si>
+    <t>Modified forest</t>
+  </si>
+  <si>
+    <t>“Base” Forest</t>
+  </si>
+  <si>
+    <t>Notes: The numbers are RMSEs on a one-month forward forecast from January 1999 to January 2020, performed by five different models. The first column refers to the modified random forest I describe in Section 3. The ARIMA model is optimized by AIC. The “base” random forest is as described in Section 2. The naïve forecast simply predicts that next month inflation will be the same as current month inflation. RMSEs for the random forest and the “base” random forest are not replicable.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +162,25 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -103,7 +190,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -120,11 +207,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -137,6 +282,90 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -51526,14 +51755,576 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F3B8E62-0567-A24F-B738-76B8EE298C37}">
+  <dimension ref="A1:N27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="19"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="12">
+        <v>1.0162899999999999</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1.029163</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.97160349999999995</v>
+      </c>
+      <c r="G5" s="12">
+        <v>1.015209</v>
+      </c>
+      <c r="H5" s="22">
+        <v>1.0257080000000001</v>
+      </c>
+      <c r="I5" s="22"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="12">
+        <v>1.0528029999999999</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1.16591</v>
+      </c>
+      <c r="F6" s="12">
+        <v>1.0922000000000001</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1.036251</v>
+      </c>
+      <c r="H6" s="21">
+        <v>1.0631930000000001</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" ht="44" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="26"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="26"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="26"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="26"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" t="s">
+        <v>6</v>
+      </c>
+      <c r="N20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1.0162899999999999</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1.029163</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.97160349999999995</v>
+      </c>
+      <c r="F21" s="12">
+        <v>1.015209</v>
+      </c>
+      <c r="G21">
+        <v>1.0257080000000001</v>
+      </c>
+      <c r="I21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="31">
+        <f>C21/$G21</f>
+        <v>0.99081804958136221</v>
+      </c>
+      <c r="K21" s="31">
+        <f t="shared" ref="K21:N22" si="0">D21/$G21</f>
+        <v>1.0033684050431506</v>
+      </c>
+      <c r="L21" s="31">
+        <f t="shared" si="0"/>
+        <v>0.94725155697332952</v>
+      </c>
+      <c r="M21" s="31">
+        <f t="shared" si="0"/>
+        <v>0.98976414340143581</v>
+      </c>
+      <c r="N21" s="31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="12">
+        <v>1.0528029999999999</v>
+      </c>
+      <c r="D22" s="12">
+        <v>1.16591</v>
+      </c>
+      <c r="E22" s="12">
+        <v>1.0922000000000001</v>
+      </c>
+      <c r="F22" s="10">
+        <v>1.036251</v>
+      </c>
+      <c r="G22">
+        <v>1.0631930000000001</v>
+      </c>
+      <c r="I22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="31">
+        <f>C22/$G22</f>
+        <v>0.99022755040712263</v>
+      </c>
+      <c r="K22" s="31">
+        <f t="shared" si="0"/>
+        <v>1.0966118098971682</v>
+      </c>
+      <c r="L22" s="31">
+        <f t="shared" si="0"/>
+        <v>1.0272829110048693</v>
+      </c>
+      <c r="M22" s="31">
+        <f t="shared" si="0"/>
+        <v>0.97465935159467754</v>
+      </c>
+      <c r="N22" s="31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B26" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B27" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF206A27-BE27-7B40-AB71-FDC0773A40EB}">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:12" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="9"/>
+      <c r="B3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="34"/>
+      <c r="B5" s="35">
+        <v>2.673159E-3</v>
+      </c>
+      <c r="C5" s="14">
+        <v>2.7167929999999999E-3</v>
+      </c>
+      <c r="D5" s="14">
+        <v>2.740606E-3</v>
+      </c>
+      <c r="E5" s="14">
+        <v>2.9361349999999999E-3</v>
+      </c>
+      <c r="F5" s="14">
+        <v>3.0884319999999999E-3</v>
+      </c>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:12" ht="44" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="B9" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="29">
+        <v>2.673159E-3</v>
+      </c>
+      <c r="C10" s="29">
+        <v>2.7167929999999999E-3</v>
+      </c>
+      <c r="D10" s="29">
+        <v>2.740606E-3</v>
+      </c>
+      <c r="E10" s="29">
+        <v>2.9361349999999999E-3</v>
+      </c>
+      <c r="F10" s="29">
+        <v>3.0884319999999999E-3</v>
+      </c>
+      <c r="H10" s="6">
+        <f>B10/$F10</f>
+        <v>0.86553921213094542</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" ref="I10:L10" si="0">C10/$F10</f>
+        <v>0.87966741699347761</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.88737780206914063</v>
+      </c>
+      <c r="K10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.95068792189693674</v>
+      </c>
+      <c r="L10" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A6:G6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A740F22-8CC2-D148-8023-2A07839888DC}">
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G1" sqref="G1:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -51583,23 +52374,23 @@
       <c r="E2" s="3">
         <v>3.0883999999999998E-3</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="6">
         <f>A2/$E2</f>
         <v>0.86556145576997812</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="6">
         <f t="shared" ref="H2:K2" si="0">B2/$E2</f>
         <v>0.87967879808314997</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="6">
         <f t="shared" si="0"/>
         <v>0.88738505374951437</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="6">
         <f t="shared" si="0"/>
         <v>0.95068643958036536</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -51620,23 +52411,23 @@
       <c r="E3" s="3">
         <v>4.1520999999999997E-3</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <f t="shared" ref="G3:G9" si="1">A3/$E3</f>
         <v>0.72018978348305684</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="6">
         <f t="shared" ref="H3:H9" si="2">B3/$E3</f>
         <v>0.74225090917848802</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="6">
         <f t="shared" ref="I3:I9" si="3">C3/$E3</f>
         <v>0.76823775920618487</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="6">
         <f t="shared" ref="J3:J9" si="4">D3/$E3</f>
         <v>0.71527660701813545</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="6">
         <f t="shared" ref="K3:K9" si="5">E3/$E3</f>
         <v>1</v>
       </c>
@@ -51657,23 +52448,23 @@
       <c r="E4" s="3">
         <v>4.1339999999999997E-3</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="6">
         <f t="shared" si="1"/>
         <v>0.69871794871794879</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="6">
         <f t="shared" si="2"/>
         <v>0.73284954039671024</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="6">
         <f t="shared" si="3"/>
         <v>0.76814223512336721</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="6">
         <f t="shared" si="4"/>
         <v>0.70060474117077898</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="6">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -51694,26 +52485,33 @@
       <c r="E5" s="3">
         <v>4.2874999999999996E-3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="6">
         <f t="shared" si="1"/>
         <v>0.70413994169096217</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="6">
         <f t="shared" si="2"/>
         <v>0.70745189504373174</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="6">
         <f t="shared" si="3"/>
         <v>0.74920116618075816</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="6">
         <f t="shared" si="4"/>
         <v>0.68403498542274066</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="6">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
@@ -51731,23 +52529,23 @@
       <c r="E7" s="3">
         <v>0.1402477</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <f t="shared" si="1"/>
         <v>1.0068699878857195</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <f t="shared" si="2"/>
         <v>0.96247567696297331</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="6">
         <f t="shared" si="3"/>
         <v>1.0173207831572282</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="6">
         <f t="shared" si="4"/>
         <v>1.0014217701965877</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="6">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -51768,23 +52566,23 @@
       <c r="E8" s="3">
         <v>0.23989489999999999</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="6">
         <f t="shared" si="1"/>
         <v>0.86876586371781983</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="6">
         <f t="shared" si="2"/>
         <v>0.92819397161006767</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="6">
         <f t="shared" si="3"/>
         <v>0.87163837163691271</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="6">
         <f t="shared" si="4"/>
         <v>0.97719543016545996</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="6">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -51805,23 +52603,23 @@
       <c r="E9" s="3">
         <v>4.0153000000000003E-3</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <f t="shared" si="1"/>
         <v>0.6176624411625532</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="6">
         <f t="shared" si="2"/>
         <v>0.32425970662217019</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="6">
         <f t="shared" si="3"/>
         <v>0.7150399721066919</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="6">
         <f t="shared" si="4"/>
         <v>0.62035215301471858</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="6">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -51865,19 +52663,19 @@
       <c r="D12">
         <v>3.0883999999999998E-3</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
         <f>A12/$D12</f>
         <v>0.87116306177956238</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="6">
         <f t="shared" ref="H12:J12" si="6">B12/$D12</f>
         <v>0.679283771532185</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="6">
         <f t="shared" si="6"/>
         <v>0.92711436342442699</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="6">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>

</xml_diff>